<commit_message>
Updated eoi bidder list export
</commit_message>
<xml_diff>
--- a/src/private/templates/eoi_bidder_list.xlsx
+++ b/src/private/templates/eoi_bidder_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/batamarbattulga/Documents/works/ot/backend/src/private/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/works/ot-backend/src/private/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>ARIBA NO: WS/CW NUMBER</t>
   </si>
@@ -52,26 +52,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> *</t>
-    </r>
-  </si>
-  <si>
-    <t>ISSUE DATE:</t>
-  </si>
-  <si>
-    <t>CLOSING DATE:</t>
-  </si>
-  <si>
     <t>VALUE FOR THIS SCOPE ONLY</t>
   </si>
   <si>
@@ -102,9 +82,6 @@
   </si>
   <si>
     <t>DATE</t>
-  </si>
-  <si>
-    <t>SOURCING MANAGER (goods/services)</t>
   </si>
   <si>
     <t>via Ariba eSign or physical signature here</t>
@@ -176,23 +153,61 @@
     <t>BIDDERS LIST</t>
   </si>
   <si>
-    <t>Revision # 5.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOURCING TEAM </t>
   </si>
   <si>
-    <t>Effective Date: 10/06/2017</t>
-  </si>
-  <si>
     <t>Page# 1</t>
+  </si>
+  <si>
+    <t>Revision #8</t>
+  </si>
+  <si>
+    <t>Effective Date: 26/01/2019</t>
+  </si>
+  <si>
+    <t>BID ISSUE DATE:</t>
+  </si>
+  <si>
+    <t>BID CLOSING DATE:</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Amartuvshin Delger</t>
+  </si>
+  <si>
+    <t>Shayne Eccles</t>
+  </si>
+  <si>
+    <t>OPERATION SOURCING MANAGER</t>
+  </si>
+  <si>
+    <t>STRATEGIC SOURCING MANAGER</t>
+  </si>
+  <si>
+    <t>Batbaatar Galsandorj</t>
+  </si>
+  <si>
+    <r>
+      <t>     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> *</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +326,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -514,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -526,9 +553,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -581,6 +605,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -686,10 +713,61 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -701,57 +779,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -761,14 +788,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1131,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="237" zoomScaleNormal="237" zoomScalePageLayoutView="237" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="237" zoomScaleNormal="237" zoomScalePageLayoutView="237" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1153,31 +1183,31 @@
       <c r="A1" s="26"/>
       <c r="B1" s="27"/>
       <c r="C1" s="49" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="50"/>
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
-      <c r="G1" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="79"/>
+      <c r="G1" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="29"/>
       <c r="C2" s="51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
       <c r="F2" s="53"/>
-      <c r="G2" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="82"/>
+      <c r="G2" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
@@ -1186,30 +1216,30 @@
       <c r="D3" s="55"/>
       <c r="E3" s="55"/>
       <c r="F3" s="56"/>
-      <c r="G3" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="17"/>
+      <c r="B4" s="16"/>
       <c r="C4"/>
       <c r="D4"/>
-      <c r="H4" s="20"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="17"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="H5" s="18"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="C6"/>
       <c r="D6"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="14"/>
       <c r="F6"/>
     </row>
     <row r="7" spans="1:9" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1223,13 +1253,13 @@
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="44"/>
-      <c r="G7" s="88" t="s">
+      <c r="G7" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="88"/>
+      <c r="H7" s="86"/>
       <c r="I7" s="48"/>
     </row>
-    <row r="8" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>3</v>
       </c>
@@ -1240,27 +1270,27 @@
       <c r="D8" s="40"/>
       <c r="E8" s="40"/>
       <c r="F8" s="41"/>
-      <c r="G8" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
+      <c r="G8" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="87"/>
+      <c r="I8" s="88"/>
     </row>
     <row r="9" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B9" s="46"/>
-      <c r="C9" s="23" t="s">
-        <v>6</v>
+      <c r="C9" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="35"/>
       <c r="G9" s="83" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H9" s="84"/>
       <c r="I9" s="85"/>
@@ -1270,7 +1300,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="38"/>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="36" t="s">
@@ -1278,11 +1308,11 @@
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="38"/>
-      <c r="G10" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="66"/>
-      <c r="I10" s="67"/>
+      <c r="G10" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -1295,7 +1325,7 @@
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12"/>
@@ -1304,66 +1334,78 @@
       <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="35"/>
-      <c r="C13" s="61"/>
+      <c r="C13" s="61" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="62"/>
       <c r="E13" s="34" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="35"/>
       <c r="H13" s="33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:9" ht="48.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B14" s="58"/>
-      <c r="C14" s="57"/>
+      <c r="C14" s="57" t="s">
+        <v>34</v>
+      </c>
       <c r="D14" s="58"/>
-      <c r="E14" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="73"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="71"/>
-    </row>
-    <row r="15" spans="1:9" ht="47.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="57"/>
+      <c r="E14" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="68"/>
+    </row>
+    <row r="15" spans="1:9" ht="48.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="57" t="s">
+        <v>38</v>
+      </c>
       <c r="D15" s="58"/>
-      <c r="E15" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="58"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E15" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="68"/>
+    </row>
+    <row r="16" spans="1:9" ht="47.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="60"/>
+      <c r="C16" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="72"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -1371,74 +1413,85 @@
       <c r="F17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:9" s="89" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="66"/>
+      <c r="H19" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="66"/>
+    </row>
+    <row r="20" spans="1:9" ht="44" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="68" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="69"/>
-      <c r="H18" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="69"/>
-    </row>
-    <row r="19" spans="1:9" ht="44" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="37">
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G3:I3"/>
@@ -1446,19 +1499,24 @@
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G10:I10"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="D9:F9"/>
@@ -1471,7 +1529,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F3"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>